<commit_message>
Recurring Desposit 14 test cases
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4733-SUBMITSAVINGS01JAN2015-DEPOSIT3000on01JAN2015-TRANSFER846on08JAN2015toLOANACCOUNTofOTHERCLIENT-2ndClient.xlsx
+++ b/Mifos Automation Excels/Client/4733-SUBMITSAVINGS01JAN2015-DEPOSIT3000on01JAN2015-TRANSFER846on08JAN2015toLOANACCOUNTofOTHERCLIENT-2ndClient.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Create Client2" sheetId="1" r:id="rId1"/>
@@ -757,7 +757,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>